<commit_message>
for scores list sort by hole group team name
</commit_message>
<xml_diff>
--- a/monster-golf-docs/monster2014/Monster2014.xlsx
+++ b/monster-golf-docs/monster2014/Monster2014.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11640" windowHeight="6690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11640" windowHeight="6690" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Flights" sheetId="4" r:id="rId1"/>
+    <sheet name="Groups" sheetId="5" r:id="rId2"/>
+    <sheet name="Missing Info" sheetId="3" r:id="rId3"/>
+    <sheet name="Everything" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="354">
   <si>
     <t>Jake</t>
   </si>
@@ -805,6 +807,288 @@
   </si>
   <si>
     <t>mike.roseleip@docusign.com</t>
+  </si>
+  <si>
+    <t>HCP</t>
+  </si>
+  <si>
+    <t>Kern Ward</t>
+  </si>
+  <si>
+    <t>Mike Stork</t>
+  </si>
+  <si>
+    <t>Randy Olson</t>
+  </si>
+  <si>
+    <t>Rick Becker</t>
+  </si>
+  <si>
+    <t>Steve Fennewald</t>
+  </si>
+  <si>
+    <t>Andy Ness</t>
+  </si>
+  <si>
+    <t>Dan Borg</t>
+  </si>
+  <si>
+    <t>Nate Bess</t>
+  </si>
+  <si>
+    <t>Travis Pitts</t>
+  </si>
+  <si>
+    <t>Brian Giesinger</t>
+  </si>
+  <si>
+    <t>Doug Wald</t>
+  </si>
+  <si>
+    <t>Kirk Redfern</t>
+  </si>
+  <si>
+    <t>Pat Evenson</t>
+  </si>
+  <si>
+    <t>Joel Van Dyk</t>
+  </si>
+  <si>
+    <t>Shawn Dumphy</t>
+  </si>
+  <si>
+    <t>Zachary Sumners</t>
+  </si>
+  <si>
+    <t>Brian Donaldson</t>
+  </si>
+  <si>
+    <t>Dewey Wald</t>
+  </si>
+  <si>
+    <t>Grant Peterson</t>
+  </si>
+  <si>
+    <t>Patti Wald</t>
+  </si>
+  <si>
+    <t>Andy Podolak</t>
+  </si>
+  <si>
+    <t>Laura Roseleip</t>
+  </si>
+  <si>
+    <t>Mike Roseleip</t>
+  </si>
+  <si>
+    <t>Mitch Mondala</t>
+  </si>
+  <si>
+    <t>Brad Epker</t>
+  </si>
+  <si>
+    <t>Clyde Gies</t>
+  </si>
+  <si>
+    <t>Jeremy Gies</t>
+  </si>
+  <si>
+    <t>Jon Gies</t>
+  </si>
+  <si>
+    <t>Barak Schneeweiss</t>
+  </si>
+  <si>
+    <t>Dwane Liuska</t>
+  </si>
+  <si>
+    <t>Marshal Hagen</t>
+  </si>
+  <si>
+    <t>Vincent Larson</t>
+  </si>
+  <si>
+    <t>Jen Callahan</t>
+  </si>
+  <si>
+    <t>John Francis</t>
+  </si>
+  <si>
+    <t>Steve Francis</t>
+  </si>
+  <si>
+    <t>Terrie Levitt</t>
+  </si>
+  <si>
+    <t>Curt Erie</t>
+  </si>
+  <si>
+    <t>Myron Irwin</t>
+  </si>
+  <si>
+    <t>Rick Levitt</t>
+  </si>
+  <si>
+    <t>Scott Hinners</t>
+  </si>
+  <si>
+    <t>Bob Cruzan</t>
+  </si>
+  <si>
+    <t>Christopher Stafford</t>
+  </si>
+  <si>
+    <t>Derek Gulbransen</t>
+  </si>
+  <si>
+    <t>Garth Billsten</t>
+  </si>
+  <si>
+    <t>Bob Holso</t>
+  </si>
+  <si>
+    <t>Dennis Wurmlinger</t>
+  </si>
+  <si>
+    <t>Jeff Wurmlinger</t>
+  </si>
+  <si>
+    <t>KT Thayer</t>
+  </si>
+  <si>
+    <t>Jake Jorde</t>
+  </si>
+  <si>
+    <t>Jeff Herberger</t>
+  </si>
+  <si>
+    <t>Jim Clark</t>
+  </si>
+  <si>
+    <t>Mike Levitt</t>
+  </si>
+  <si>
+    <t>Beau Stonefield</t>
+  </si>
+  <si>
+    <t>Dan Luoma</t>
+  </si>
+  <si>
+    <t>Mike Borreson</t>
+  </si>
+  <si>
+    <t>Ryan Thomas</t>
+  </si>
+  <si>
+    <t>Aaron Wald</t>
+  </si>
+  <si>
+    <t>Jon Hanson</t>
+  </si>
+  <si>
+    <t>Paul Plemel</t>
+  </si>
+  <si>
+    <t>Steve Wald</t>
+  </si>
+  <si>
+    <t>Darryl Podolak</t>
+  </si>
+  <si>
+    <t>Dick Dadisman</t>
+  </si>
+  <si>
+    <t>Steven Ehase</t>
+  </si>
+  <si>
+    <t>Talbet Sumners</t>
+  </si>
+  <si>
+    <t>Chad Bodine</t>
+  </si>
+  <si>
+    <t>Jeff Wald</t>
+  </si>
+  <si>
+    <t>Mike Schuette</t>
+  </si>
+  <si>
+    <t>Todd Bodine</t>
+  </si>
+  <si>
+    <t>Ian Quarders</t>
+  </si>
+  <si>
+    <t>John Blackburn</t>
+  </si>
+  <si>
+    <t>Scott Hanson</t>
+  </si>
+  <si>
+    <t>Wayne Podolak</t>
+  </si>
+  <si>
+    <t>Brad Ahrens</t>
+  </si>
+  <si>
+    <t>Brad Krogstad</t>
+  </si>
+  <si>
+    <t>Jason Bartsch</t>
+  </si>
+  <si>
+    <t>Troy Grondahl</t>
+  </si>
+  <si>
+    <t>Jeff Haseleu</t>
+  </si>
+  <si>
+    <t>Michael Benson</t>
+  </si>
+  <si>
+    <t>Neil Hefta</t>
+  </si>
+  <si>
+    <t>Scott Anderson</t>
+  </si>
+  <si>
+    <t>Al Loftis</t>
+  </si>
+  <si>
+    <t>Brian Burbank</t>
+  </si>
+  <si>
+    <t>Greg Robertson</t>
+  </si>
+  <si>
+    <t>Matt Smith</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>Starting Hole</t>
+  </si>
+  <si>
+    <t>HCP2</t>
+  </si>
+  <si>
+    <t>Email2</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>First2</t>
+  </si>
+  <si>
+    <t>Last2</t>
   </si>
 </sst>
 </file>
@@ -814,7 +1098,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,8 +1120,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -854,8 +1167,19 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -863,13 +1187,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -881,16 +1225,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     </dxf>
@@ -909,6 +1280,9 @@
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -923,6 +1297,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J43" totalsRowShown="0">
+  <autoFilter ref="A1:J43"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="TeamHCP"/>
+    <tableColumn id="2" name="Flight"/>
+    <tableColumn id="3" name="First"/>
+    <tableColumn id="4" name="Last"/>
+    <tableColumn id="5" name="HCP"/>
+    <tableColumn id="6" name="Email"/>
+    <tableColumn id="7" name="First2"/>
+    <tableColumn id="8" name="Last2"/>
+    <tableColumn id="9" name="HCP2"/>
+    <tableColumn id="10" name="Email2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AE43" totalsRowShown="0">
   <autoFilter ref="A1:AE43"/>
   <sortState ref="A2:AD43">
@@ -931,8 +1324,8 @@
   </sortState>
   <tableColumns count="31">
     <tableColumn id="1" name="TeamId"/>
-    <tableColumn id="27" name="Flight" dataDxfId="0"/>
-    <tableColumn id="2" name="TeamHCP"/>
+    <tableColumn id="27" name="TeamHCP" dataDxfId="6"/>
+    <tableColumn id="2" name="Flight"/>
     <tableColumn id="3" name="UserId"/>
     <tableColumn id="4" name="FirstName"/>
     <tableColumn id="5" name="LastName"/>
@@ -944,9 +1337,9 @@
     <tableColumn id="11" name="TourneyScoresR2HCP"/>
     <tableColumn id="28" name="Email"/>
     <tableColumn id="30" name="MobileEmail"/>
-    <tableColumn id="12" name="HCP Location" dataDxfId="6"/>
-    <tableColumn id="13" name="DateOfRound" dataDxfId="5"/>
-    <tableColumn id="14" name="DateEntered" dataDxfId="4"/>
+    <tableColumn id="12" name="HCP Location" dataDxfId="5"/>
+    <tableColumn id="13" name="DateOfRound" dataDxfId="4"/>
+    <tableColumn id="14" name="DateEntered" dataDxfId="3"/>
     <tableColumn id="15" name="UserID2"/>
     <tableColumn id="16" name="FirstName3"/>
     <tableColumn id="17" name="LastName4"/>
@@ -958,9 +1351,9 @@
     <tableColumn id="23" name="TourneyScoresR2HCP10"/>
     <tableColumn id="29" name="Email11"/>
     <tableColumn id="31" name="MobileEmail12"/>
-    <tableColumn id="24" name="HCP Location13" dataDxfId="3"/>
-    <tableColumn id="25" name="DateOfRound14" dataDxfId="2"/>
-    <tableColumn id="26" name="DateEntered15" dataDxfId="1"/>
+    <tableColumn id="24" name="HCP Location13" dataDxfId="2"/>
+    <tableColumn id="25" name="DateOfRound14" dataDxfId="1"/>
+    <tableColumn id="26" name="DateEntered15" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1229,16 +1622,3167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>352</v>
+      </c>
+      <c r="H1" t="s">
+        <v>353</v>
+      </c>
+      <c r="I1" t="s">
+        <v>348</v>
+      </c>
+      <c r="J1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9.6</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9.9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>14.8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16.3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16.8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>18.5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>22.7</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>189</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>23.2</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>23.6</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>25.8</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>197</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17">
+        <v>15</v>
+      </c>
+      <c r="J17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>26.1</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>26.9</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19">
+        <v>13</v>
+      </c>
+      <c r="J19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>28.9</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>203</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>28.9</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30.1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>207</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>209</v>
+      </c>
+      <c r="G23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>32.5</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>33.1</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25">
+        <v>18</v>
+      </c>
+      <c r="G25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>33.5</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>213</v>
+      </c>
+      <c r="G26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
+        <v>214</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27">
+        <v>14</v>
+      </c>
+      <c r="J27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>35.5</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>216</v>
+      </c>
+      <c r="G28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28">
+        <v>23</v>
+      </c>
+      <c r="J28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I29">
+        <v>23</v>
+      </c>
+      <c r="J29" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>38.1</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>220</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30">
+        <v>17</v>
+      </c>
+      <c r="J30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>222</v>
+      </c>
+      <c r="G31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31">
+        <v>28</v>
+      </c>
+      <c r="J31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>224</v>
+      </c>
+      <c r="G32" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" t="s">
+        <v>109</v>
+      </c>
+      <c r="I32">
+        <v>14</v>
+      </c>
+      <c r="J32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>42.4</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33">
+        <v>23</v>
+      </c>
+      <c r="F33" t="s">
+        <v>226</v>
+      </c>
+      <c r="G33" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33">
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>42.7</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34">
+        <v>23</v>
+      </c>
+      <c r="F34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G34" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34">
+        <v>20</v>
+      </c>
+      <c r="J34" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>44.6</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35">
+        <v>24</v>
+      </c>
+      <c r="F35" t="s">
+        <v>228</v>
+      </c>
+      <c r="G35" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35">
+        <v>21</v>
+      </c>
+      <c r="J35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>49.1</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36">
+        <v>31</v>
+      </c>
+      <c r="F36" t="s">
+        <v>232</v>
+      </c>
+      <c r="G36" t="s">
+        <v>120</v>
+      </c>
+      <c r="H36" t="s">
+        <v>121</v>
+      </c>
+      <c r="I36">
+        <v>18</v>
+      </c>
+      <c r="J36" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>49.7</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>234</v>
+      </c>
+      <c r="G37" t="s">
+        <v>126</v>
+      </c>
+      <c r="H37" t="s">
+        <v>127</v>
+      </c>
+      <c r="I37">
+        <v>32</v>
+      </c>
+      <c r="J37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>50.4</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38">
+        <v>17</v>
+      </c>
+      <c r="F38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G38" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" t="s">
+        <v>130</v>
+      </c>
+      <c r="I38">
+        <v>34</v>
+      </c>
+      <c r="J38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>51</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39">
+        <v>23</v>
+      </c>
+      <c r="F39" t="s">
+        <v>238</v>
+      </c>
+      <c r="G39" t="s">
+        <v>132</v>
+      </c>
+      <c r="H39" t="s">
+        <v>133</v>
+      </c>
+      <c r="I39">
+        <v>28</v>
+      </c>
+      <c r="J39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>52.7</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40">
+        <v>23</v>
+      </c>
+      <c r="F40" t="s">
+        <v>240</v>
+      </c>
+      <c r="G40" t="s">
+        <v>123</v>
+      </c>
+      <c r="H40" t="s">
+        <v>124</v>
+      </c>
+      <c r="I40">
+        <v>30</v>
+      </c>
+      <c r="J40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>53.8</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>242</v>
+      </c>
+      <c r="G41" t="s">
+        <v>134</v>
+      </c>
+      <c r="H41" t="s">
+        <v>135</v>
+      </c>
+      <c r="I41">
+        <v>35</v>
+      </c>
+      <c r="J41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>59.9</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" t="s">
+        <v>137</v>
+      </c>
+      <c r="E42">
+        <v>30</v>
+      </c>
+      <c r="F42" t="s">
+        <v>244</v>
+      </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" t="s">
+        <v>138</v>
+      </c>
+      <c r="I42">
+        <v>30</v>
+      </c>
+      <c r="J42" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>74.2</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43">
+        <v>39</v>
+      </c>
+      <c r="F43" t="s">
+        <v>246</v>
+      </c>
+      <c r="G43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>140</v>
+      </c>
+      <c r="I43">
+        <v>35</v>
+      </c>
+      <c r="J43" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="15">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="G2" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="15">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="G3" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" s="15">
+        <v>20</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G4" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="15">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="G5" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="9">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="16">
+        <v>15</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="G6" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="16">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="G7" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="16">
+        <v>31</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="G8" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D9" s="16">
+        <v>18</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G9" s="16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="15">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G10" s="15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" s="15">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="G11" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="15">
+        <v>14</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="G12" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" s="15">
+        <v>15</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G13" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="9">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" s="16">
+        <v>21</v>
+      </c>
+      <c r="E14" s="9">
+        <v>4</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="G14" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" s="16">
+        <v>4</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="G15" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D16" s="16">
+        <v>11</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="G16" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" s="16">
+        <v>6</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="G17" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="8">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D18" s="15">
+        <v>30</v>
+      </c>
+      <c r="E18" s="8">
+        <v>5</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="G18" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" s="15">
+        <v>11</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G19" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" s="15">
+        <v>30</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="G20" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D21" s="15">
+        <v>28</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="G21" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="9">
+        <v>6</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" s="16">
+        <v>19</v>
+      </c>
+      <c r="E22" s="9">
+        <v>6</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="G22" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D23" s="16">
+        <v>39</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="G23" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D24" s="16">
+        <v>35</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="G24" s="16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D25" s="16">
+        <v>35</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="G25" s="16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="8">
+        <v>7</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D26" s="15">
+        <v>23</v>
+      </c>
+      <c r="E26" s="8">
+        <v>7</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G26" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" s="15">
+        <v>23</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="G27" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D28" s="15">
+        <v>19</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="G28" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" s="15">
+        <v>12</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="G29" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="9">
+        <v>8</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D30" s="16">
+        <v>13</v>
+      </c>
+      <c r="E30" s="9">
+        <v>8</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="G30" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D31" s="16">
+        <v>24</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G31" s="16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D32" s="16">
+        <v>21</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="G32" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" s="16">
+        <v>23</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G33" s="16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="8">
+        <v>9</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D34" s="15">
+        <v>18</v>
+      </c>
+      <c r="E34" s="8">
+        <v>9</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G34" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D35" s="15">
+        <v>22</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="G35" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="D36" s="15">
+        <v>10</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="G36" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D37" s="15">
+        <v>15</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="G37" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="9">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D38" s="16">
+        <v>13</v>
+      </c>
+      <c r="E38" s="9">
+        <v>10</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G38" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D39" s="16">
+        <v>14</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="G39" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D40" s="16">
+        <v>15</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="G40" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D41" s="16">
+        <v>8</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="G41" s="16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="8">
+        <v>11</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D42" s="15">
+        <v>23</v>
+      </c>
+      <c r="E42" s="8">
+        <v>11</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="G42" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D43" s="15">
+        <v>32</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G43" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D44" s="15">
+        <v>30</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G44" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D45" s="15">
+        <v>18</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G45" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="9">
+        <v>12</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="16">
+        <v>11</v>
+      </c>
+      <c r="E46" s="9">
+        <v>12</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="G46" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D47" s="16">
+        <v>15</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G47" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D48" s="16">
+        <v>14</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="G48" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D49" s="16">
+        <v>20</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G49" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="8">
+        <v>13</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D50" s="15">
+        <v>2</v>
+      </c>
+      <c r="E50" s="8">
+        <v>13</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G50" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D51" s="15">
+        <v>4</v>
+      </c>
+      <c r="E51" s="8"/>
+      <c r="F51" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="G51" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D52" s="15">
+        <v>3</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="G52" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="D53" s="15">
+        <v>5</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="G53" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="9">
+        <v>14</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D54" s="16">
+        <v>10</v>
+      </c>
+      <c r="E54" s="9">
+        <v>14</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G54" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D55" s="16">
+        <v>34</v>
+      </c>
+      <c r="E55" s="9"/>
+      <c r="F55" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="G55" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D56" s="16">
+        <v>7</v>
+      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="G56" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D57" s="16">
+        <v>17</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="G57" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="8">
+        <v>15</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D58" s="15">
+        <v>8</v>
+      </c>
+      <c r="E58" s="8">
+        <v>15</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="G58" s="15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D59" s="15">
+        <v>2</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G59" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="D60" s="15">
+        <v>11</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="G60" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D61" s="15">
+        <v>7</v>
+      </c>
+      <c r="E61" s="8"/>
+      <c r="F61" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="G61" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="9">
+        <v>16</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D62" s="16">
+        <v>27</v>
+      </c>
+      <c r="E62" s="9">
+        <v>16</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="G62" s="16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D63" s="16">
+        <v>14</v>
+      </c>
+      <c r="E63" s="9"/>
+      <c r="F63" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="G63" s="16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D64" s="16">
+        <v>5</v>
+      </c>
+      <c r="E64" s="9"/>
+      <c r="F64" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G64" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D65" s="16">
+        <v>11</v>
+      </c>
+      <c r="E65" s="9"/>
+      <c r="F65" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="G65" s="16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="8">
+        <v>17</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D66" s="15">
+        <v>7</v>
+      </c>
+      <c r="E66" s="8">
+        <v>17</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="G66" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D67" s="15">
+        <v>7</v>
+      </c>
+      <c r="E67" s="8"/>
+      <c r="F67" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="G67" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D68" s="15">
+        <v>16</v>
+      </c>
+      <c r="E68" s="8"/>
+      <c r="F68" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="G68" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D69" s="15">
+        <v>11</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="G69" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+      <c r="B70" s="9">
+        <v>18</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D70" s="16">
+        <v>14</v>
+      </c>
+      <c r="E70" s="9">
+        <v>18</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="G70" s="16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D71" s="16">
+        <v>9</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G71" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="D72" s="16">
+        <v>16</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="G72" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D73" s="16">
+        <v>15</v>
+      </c>
+      <c r="E73" s="9"/>
+      <c r="F73" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="G73" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="8">
+        <v>1</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="D74" s="15">
+        <v>16</v>
+      </c>
+      <c r="E74" s="8">
+        <v>1</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="G74" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="10"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D75" s="15">
+        <v>5</v>
+      </c>
+      <c r="E75" s="8"/>
+      <c r="F75" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="G75" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D76" s="15">
+        <v>10</v>
+      </c>
+      <c r="E76" s="8"/>
+      <c r="F76" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="G76" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="D77" s="15">
+        <v>8</v>
+      </c>
+      <c r="E77" s="8"/>
+      <c r="F77" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G77" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="11"/>
+      <c r="B78" s="9">
+        <v>2</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D78" s="16">
+        <v>7</v>
+      </c>
+      <c r="E78" s="9">
+        <v>2</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="G78" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="11"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D79" s="16">
+        <v>23</v>
+      </c>
+      <c r="E79" s="9"/>
+      <c r="F79" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="G79" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="11"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D80" s="16">
+        <v>20</v>
+      </c>
+      <c r="E80" s="9"/>
+      <c r="F80" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="G80" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D81" s="16">
+        <v>12</v>
+      </c>
+      <c r="E81" s="9"/>
+      <c r="F81" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="G81" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="10"/>
+      <c r="B82" s="8">
+        <v>3</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D82" s="15">
+        <v>28</v>
+      </c>
+      <c r="E82" s="8">
+        <v>3</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="G82" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="10"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D83" s="15">
+        <v>23</v>
+      </c>
+      <c r="E83" s="8"/>
+      <c r="F83" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="G83" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="10"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D84" s="15">
+        <v>16</v>
+      </c>
+      <c r="E84" s="8"/>
+      <c r="F84" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G84" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="10"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D85" s="15">
+        <v>18</v>
+      </c>
+      <c r="E85" s="8"/>
+      <c r="F85" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="G85" s="15">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E22:E25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4">
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9">
+        <v>22.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="D2:F10">
+    <sortCondition ref="D2:D10"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1262,10 +4806,10 @@
         <v>141</v>
       </c>
       <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" t="s">
         <v>142</v>
-      </c>
-      <c r="C1" t="s">
-        <v>167</v>
       </c>
       <c r="D1" t="s">
         <v>143</v>
@@ -5215,173 +8759,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="A1:F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2">
-        <v>15.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4">
-        <v>31.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F5">
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7">
-        <v>26.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10">
-        <v>22.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="D2:F10">
-    <sortCondition ref="D2:D10"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>